<commit_message>
programada a coleta de dados VDE e organização das tabelas derivadas da fonte
</commit_message>
<xml_diff>
--- a/Data/g19.1.xlsx
+++ b/Data/g19.1.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,12 +441,12 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Ano</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Variável</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Ano</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -463,180 +463,168 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>Brasil</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Homicídio doloso</t>
+          <t>01/01/2017</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>01-01-2019</t>
+          <t>Homicídio doloso</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>33.98183894689783</v>
-      </c>
-      <c r="E2" t="n">
-        <v>4</v>
-      </c>
+        <v>32.89455525672006</v>
+      </c>
+      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>Brasil</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Homicídio doloso</t>
+          <t>01/01/2018</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>01-01-2020</t>
+          <t>Homicídio doloso</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>33.80084379937774</v>
-      </c>
-      <c r="E3" t="n">
-        <v>6</v>
-      </c>
+        <v>29.92000675669447</v>
+      </c>
+      <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>Brasil</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Homicídio doloso</t>
+          <t>01/01/2019</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>01-01-2021</t>
+          <t>Homicídio doloso</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>24.52484248897287</v>
-      </c>
-      <c r="E4" t="n">
-        <v>14</v>
-      </c>
+        <v>22.78123160802507</v>
+      </c>
+      <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>Brasil</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Homicídio doloso</t>
+          <t>01/01/2020</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>01-01-2022</t>
+          <t>Homicídio doloso</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>25.3393206528133</v>
-      </c>
-      <c r="E5" t="n">
-        <v>12</v>
-      </c>
+        <v>23.95462631156656</v>
+      </c>
+      <c r="E5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>Brasil</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Homicídio doloso</t>
+          <t>01/01/2021</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>01-01-2023</t>
+          <t>Homicídio doloso</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>19.59272471905028</v>
-      </c>
-      <c r="E6" t="n">
-        <v>19</v>
-      </c>
+        <v>22.45847761979459</v>
+      </c>
+      <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>Brasil</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Homicídio doloso</t>
+          <t>01/01/2022</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>01-01-2024</t>
+          <t>Homicídio doloso</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>3.936644458562066</v>
-      </c>
-      <c r="E7" t="n">
-        <v>17</v>
-      </c>
+        <v>21.82561212792709</v>
+      </c>
+      <c r="E7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Nordeste</t>
+          <t>Brasil</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Homicídio doloso</t>
+          <t>01/01/2023</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>01-01-2019</t>
+          <t>Homicídio doloso</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>27.68956400713319</v>
+        <v>20.91732437986478</v>
       </c>
       <c r="E8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Nordeste</t>
+          <t>Brasil</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Homicídio doloso</t>
+          <t>01/01/2024</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>01-01-2020</t>
+          <t>Homicídio doloso</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>33.31082275547983</v>
+        <v>18.61443649398527</v>
       </c>
       <c r="E9" t="inlineStr"/>
     </row>
@@ -648,16 +636,16 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Homicídio doloso</t>
+          <t>01/01/2017</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>01-01-2021</t>
+          <t>Homicídio doloso</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>30.07686405680707</v>
+        <v>41.76396000036527</v>
       </c>
       <c r="E10" t="inlineStr"/>
     </row>
@@ -669,16 +657,16 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Homicídio doloso</t>
+          <t>01/01/2018</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>01-01-2022</t>
+          <t>Homicídio doloso</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>29.19465300537867</v>
+        <v>35.03400939047036</v>
       </c>
       <c r="E11" t="inlineStr"/>
     </row>
@@ -690,16 +678,16 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Homicídio doloso</t>
+          <t>01/01/2019</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>01-01-2023</t>
+          <t>Homicídio doloso</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>27.77997537784609</v>
+        <v>26.49153069038045</v>
       </c>
       <c r="E12" t="inlineStr"/>
     </row>
@@ -711,144 +699,286 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Homicídio doloso</t>
+          <t>01/01/2020</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>01-01-2024</t>
+          <t>Homicídio doloso</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>6.597172346461076</v>
+        <v>31.7167489266386</v>
       </c>
       <c r="E13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Brasil</t>
+          <t>Nordeste</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Homicídio doloso</t>
+          <t>01/01/2021</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>01-01-2019</t>
+          <t>Homicídio doloso</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>24.3495071243073</v>
+        <v>28.49517714923115</v>
       </c>
       <c r="E14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Brasil</t>
+          <t>Nordeste</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Homicídio doloso</t>
+          <t>01/01/2022</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>01-01-2020</t>
+          <t>Homicídio doloso</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>25.13767376884837</v>
+        <v>27.52826693045831</v>
       </c>
       <c r="E15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Brasil</t>
+          <t>Nordeste</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Homicídio doloso</t>
+          <t>01/01/2023</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>01-01-2021</t>
+          <t>Homicídio doloso</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>23.95295301796192</v>
+        <v>26.11187036839209</v>
       </c>
       <c r="E16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Brasil</t>
+          <t>Nordeste</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Homicídio doloso</t>
+          <t>01/01/2024</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>01-01-2022</t>
+          <t>Homicídio doloso</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>23.3865038705044</v>
+        <v>24.76353685797129</v>
       </c>
       <c r="E17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Brasil</t>
+          <t>Sergipe</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Homicídio doloso</t>
+          <t>01/01/2017</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>01-01-2023</t>
+          <t>Homicídio doloso</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>22.57652783572015</v>
-      </c>
-      <c r="E18" t="inlineStr"/>
+        <v>48.77581995210135</v>
+      </c>
+      <c r="E18" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Brasil</t>
+          <t>Sergipe</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Homicídio doloso</t>
+          <t>01/01/2018</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>01-01-2024</t>
+          <t>Homicídio doloso</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>5.057776330433875</v>
-      </c>
-      <c r="E19" t="inlineStr"/>
+        <v>40.90755069112692</v>
+      </c>
+      <c r="E19" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Homicídio doloso</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>32.66776922200251</v>
+      </c>
+      <c r="E20" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>01/01/2020</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Homicídio doloso</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>32.21171592285057</v>
+      </c>
+      <c r="E21" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>01/01/2021</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Homicídio doloso</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>23.17538722565815</v>
+      </c>
+      <c r="E22" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>01/01/2022</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Homicídio doloso</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>23.75055135208496</v>
+      </c>
+      <c r="E23" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>01/01/2023</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Homicídio doloso</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>18.30463713266065</v>
+      </c>
+      <c r="E24" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Homicídio doloso</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>14.82574116177014</v>
+      </c>
+      <c r="E25" t="n">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
anulação da regra que removia anos com dados faltantes e adição de coluna que indica se há dados faltantes
</commit_message>
<xml_diff>
--- a/Data/g19.1.xlsx
+++ b/Data/g19.1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,6 +459,11 @@
           <t>Posição relativamente às demais UF</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Faltam dados para todos os Estados</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -468,7 +473,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>01/01/2017</t>
+          <t>01/01/2015</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -477,9 +482,12 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>32.89455525672006</v>
+        <v>27.28839008256385</v>
       </c>
       <c r="E2" t="inlineStr"/>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -489,7 +497,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>01/01/2018</t>
+          <t>01/01/2016</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -498,9 +506,12 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>29.92000675669447</v>
+        <v>30.05887666703984</v>
       </c>
       <c r="E3" t="inlineStr"/>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -510,7 +521,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>01/01/2019</t>
+          <t>01/01/2017</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -519,9 +530,12 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>22.78123160802507</v>
+        <v>32.89455525672006</v>
       </c>
       <c r="E4" t="inlineStr"/>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -531,7 +545,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>01/01/2020</t>
+          <t>01/01/2018</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -540,9 +554,12 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>23.95462631156656</v>
+        <v>29.92000675669447</v>
       </c>
       <c r="E5" t="inlineStr"/>
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -552,7 +569,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>01/01/2021</t>
+          <t>01/01/2019</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -561,9 +578,12 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>22.45847761979459</v>
+        <v>22.78123160802507</v>
       </c>
       <c r="E6" t="inlineStr"/>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -573,7 +593,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>01/01/2022</t>
+          <t>01/01/2020</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -582,9 +602,12 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>21.82561212792709</v>
+        <v>23.95462631156656</v>
       </c>
       <c r="E7" t="inlineStr"/>
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -594,7 +617,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>01/01/2023</t>
+          <t>01/01/2021</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -603,9 +626,12 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>20.91732437986478</v>
+        <v>22.45847761979459</v>
       </c>
       <c r="E8" t="inlineStr"/>
+      <c r="F8" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -615,7 +641,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>01/01/2024</t>
+          <t>01/01/2022</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -624,19 +650,22 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>18.61443649398527</v>
+        <v>21.82561212792709</v>
       </c>
       <c r="E9" t="inlineStr"/>
+      <c r="F9" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Nordeste</t>
+          <t>Brasil</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>01/01/2017</t>
+          <t>01/01/2023</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -645,19 +674,22 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>41.76396000036527</v>
+        <v>20.91732437986478</v>
       </c>
       <c r="E10" t="inlineStr"/>
+      <c r="F10" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Nordeste</t>
+          <t>Brasil</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>01/01/2018</t>
+          <t>01/01/2024</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -666,9 +698,12 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>35.03400939047036</v>
+        <v>18.61443649398527</v>
       </c>
       <c r="E11" t="inlineStr"/>
+      <c r="F11" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -678,7 +713,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>01/01/2019</t>
+          <t>01/01/2015</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -687,9 +722,12 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>26.49153069038045</v>
+        <v>38.83151646101115</v>
       </c>
       <c r="E12" t="inlineStr"/>
+      <c r="F12" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -699,7 +737,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>01/01/2020</t>
+          <t>01/01/2016</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -708,9 +746,12 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>31.7167489266386</v>
+        <v>40.38565884059511</v>
       </c>
       <c r="E13" t="inlineStr"/>
+      <c r="F13" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -720,7 +761,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>01/01/2021</t>
+          <t>01/01/2017</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -729,9 +770,12 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>28.49517714923115</v>
+        <v>41.76396000036527</v>
       </c>
       <c r="E14" t="inlineStr"/>
+      <c r="F14" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -741,7 +785,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>01/01/2022</t>
+          <t>01/01/2018</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -750,9 +794,12 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>27.52826693045831</v>
+        <v>35.03400939047036</v>
       </c>
       <c r="E15" t="inlineStr"/>
+      <c r="F15" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -762,7 +809,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>01/01/2023</t>
+          <t>01/01/2019</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -771,9 +818,12 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>26.11187036839209</v>
+        <v>26.49153069038045</v>
       </c>
       <c r="E16" t="inlineStr"/>
+      <c r="F16" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -783,7 +833,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>01/01/2024</t>
+          <t>01/01/2020</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -792,19 +842,22 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>24.76353685797129</v>
+        <v>31.7167489266386</v>
       </c>
       <c r="E17" t="inlineStr"/>
+      <c r="F17" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>Nordeste</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>01/01/2017</t>
+          <t>01/01/2021</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -813,21 +866,22 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>48.77581995210135</v>
-      </c>
-      <c r="E18" t="n">
-        <v>6</v>
+        <v>28.49517714923115</v>
+      </c>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>Nordeste</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>01/01/2018</t>
+          <t>01/01/2022</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -836,21 +890,22 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>40.90755069112692</v>
-      </c>
-      <c r="E19" t="n">
-        <v>7</v>
+        <v>27.52826693045831</v>
+      </c>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>Nordeste</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>01/01/2019</t>
+          <t>01/01/2023</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -859,21 +914,22 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>32.66776922200251</v>
-      </c>
-      <c r="E20" t="n">
-        <v>4</v>
+        <v>26.11187036839209</v>
+      </c>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>Nordeste</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>01/01/2020</t>
+          <t>01/01/2024</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -882,10 +938,11 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>32.21171592285057</v>
-      </c>
-      <c r="E21" t="n">
-        <v>6</v>
+        <v>24.76353685797129</v>
+      </c>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -896,7 +953,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>01/01/2021</t>
+          <t>01/01/2015</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -905,10 +962,13 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>23.17538722565815</v>
+        <v>53.95512251106057</v>
       </c>
       <c r="E22" t="n">
-        <v>14</v>
+        <v>1</v>
+      </c>
+      <c r="F22" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="23">
@@ -919,7 +979,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>01/01/2022</t>
+          <t>01/01/2016</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -928,10 +988,13 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>23.75055135208496</v>
+        <v>58.37831652311978</v>
       </c>
       <c r="E23" t="n">
-        <v>13</v>
+        <v>1</v>
+      </c>
+      <c r="F23" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="24">
@@ -942,7 +1005,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>01/01/2023</t>
+          <t>01/01/2017</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -951,10 +1014,13 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>18.30463713266065</v>
+        <v>48.77581995210135</v>
       </c>
       <c r="E24" t="n">
-        <v>19</v>
+        <v>6</v>
+      </c>
+      <c r="F24" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -965,19 +1031,178 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
+          <t>01/01/2018</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Homicídio doloso</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>40.90755069112692</v>
+      </c>
+      <c r="E25" t="n">
+        <v>7</v>
+      </c>
+      <c r="F25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Homicídio doloso</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>32.66776922200251</v>
+      </c>
+      <c r="E26" t="n">
+        <v>4</v>
+      </c>
+      <c r="F26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>01/01/2020</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Homicídio doloso</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>32.21171592285057</v>
+      </c>
+      <c r="E27" t="n">
+        <v>6</v>
+      </c>
+      <c r="F27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>01/01/2021</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Homicídio doloso</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>23.17538722565815</v>
+      </c>
+      <c r="E28" t="n">
+        <v>14</v>
+      </c>
+      <c r="F28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>01/01/2022</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Homicídio doloso</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>23.75055135208496</v>
+      </c>
+      <c r="E29" t="n">
+        <v>13</v>
+      </c>
+      <c r="F29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>01/01/2023</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Homicídio doloso</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>18.30463713266065</v>
+      </c>
+      <c r="E30" t="n">
+        <v>19</v>
+      </c>
+      <c r="F30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
           <t>01/01/2024</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Homicídio doloso</t>
-        </is>
-      </c>
-      <c r="D25" t="n">
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Homicídio doloso</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
         <v>14.82574116177014</v>
       </c>
-      <c r="E25" t="n">
+      <c r="E31" t="n">
         <v>17</v>
+      </c>
+      <c r="F31" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>